<commit_message>
Still slowly trying to add features to freeflux Starting to do ODE analysis coding
</commit_message>
<xml_diff>
--- a/models/synechocystis/experimental_data/reactions.xlsx
+++ b/models/synechocystis/experimental_data/reactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwu\Desktop\Software\FreeFlux\github\freeflux-0.3.4\models\synechocystis\experimental_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilithflint/Desktop/MFA/MFA/models/synechocystis/experimental_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6380889E-4DFD-4131-95A0-33B4B961C46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BE95B6-5240-0442-8F14-A3B5B2B2C9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="780" windowWidth="21600" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="135">
   <si>
     <t>#reaction_ID</t>
   </si>
@@ -434,6 +434,15 @@
   </si>
   <si>
     <t>#Dilution</t>
+  </si>
+  <si>
+    <t>localization</t>
+  </si>
+  <si>
+    <t>cyt</t>
+  </si>
+  <si>
+    <t>#Measurement</t>
   </si>
 </sst>
 </file>
@@ -486,12 +495,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,21 +780,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:D60"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -799,13 +807,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -818,8 +829,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -832,8 +846,11 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>68</v>
       </c>
@@ -846,8 +863,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -860,8 +880,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
@@ -874,8 +897,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>71</v>
       </c>
@@ -888,8 +914,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
@@ -902,8 +931,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>73</v>
       </c>
@@ -916,8 +948,11 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -930,13 +965,16 @@
       <c r="D11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -949,8 +987,11 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -963,8 +1004,11 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -977,8 +1021,11 @@
       <c r="D15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -991,8 +1038,11 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1005,8 +1055,11 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1019,8 +1072,11 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>81</v>
       </c>
@@ -1033,8 +1089,11 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -1047,8 +1106,11 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1061,8 +1123,11 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1075,8 +1140,11 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1089,13 +1157,16 @@
       <c r="D23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -1108,8 +1179,11 @@
       <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -1122,8 +1196,11 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -1136,8 +1213,11 @@
       <c r="D27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>89</v>
       </c>
@@ -1150,8 +1230,11 @@
       <c r="D28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -1164,8 +1247,11 @@
       <c r="D29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -1178,8 +1264,11 @@
       <c r="D30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -1192,13 +1281,17 @@
       <c r="D31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1211,8 +1304,11 @@
       <c r="D33" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>94</v>
       </c>
@@ -1225,13 +1321,16 @@
       <c r="D34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
@@ -1244,8 +1343,11 @@
       <c r="D36" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>96</v>
       </c>
@@ -1258,13 +1360,16 @@
       <c r="D37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>97</v>
       </c>
@@ -1277,8 +1382,11 @@
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>98</v>
       </c>
@@ -1291,8 +1399,11 @@
       <c r="D40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -1305,8 +1416,11 @@
       <c r="D41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -1319,8 +1433,11 @@
       <c r="D42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>101</v>
       </c>
@@ -1333,8 +1450,11 @@
       <c r="D43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
@@ -1342,7 +1462,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>102</v>
       </c>
@@ -1355,13 +1475,16 @@
       <c r="D45" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -1375,177 +1498,218 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>121</v>
       </c>
-      <c r="D49" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" t="s">
         <v>107</v>
       </c>
-      <c r="D51" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>122</v>
       </c>
-      <c r="D52" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>112</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>114</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" t="s">
         <v>125</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" t="s">
         <v>124</v>
       </c>
-      <c r="D56" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" t="s">
         <v>124</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" t="s">
         <v>107</v>
       </c>
-      <c r="D57" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>118</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" t="s">
         <v>126</v>
       </c>
-      <c r="D59" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>119</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" t="s">
         <v>107</v>
       </c>
-      <c r="D60" s="4">
-        <v>0</v>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>